<commit_message>
fixed dataset accession and year
</commit_message>
<xml_diff>
--- a/data_exploration/CRISPR/crispr_studies.xlsx
+++ b/data_exploration/CRISPR/crispr_studies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zakirov/Documents/GitHub/PerturbationCatalogue/data_exploration/CRISPR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA10BBE-A146-F64B-A548-46357FC03E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23162C9-4BC0-764D-A702-C70E7795C2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="2440" windowWidth="28040" windowHeight="17440" xr2:uid="{65AE61D5-2EF1-1F4C-8D97-BC1AA3C27BF4}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="228">
   <si>
     <t>dataset_id</t>
   </si>
@@ -391,9 +391,6 @@
     <t>custom</t>
   </si>
   <si>
-    <t>[{"dataset_accession": null, "dataset_uri": null, "dataset_description": null, "dataset_file_name": null}]</t>
-  </si>
-  <si>
     <t>biogrid_2362</t>
   </si>
   <si>
@@ -481,9 +478,6 @@
     <t>A genome-scale pooled CRISPRi screen to identify genes essential for cell growth in K562 cells. A library of 206,421 sgRNAs (targeting 15,977 genes with 10 sgRNAs/TSS) was used in dCas9-KRAB expressing cells, and sgRNA frequencies were measured after 10 days of growth to identify depleted sgRNAs.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Jonathan S. Weissman</t>
-  </si>
-  <si>
     <t>Luke A. Gilbert</t>
   </si>
   <si>
@@ -640,9 +634,6 @@
     <t>MaGeCK</t>
   </si>
   <si>
-    <t>[{"dataset_accession": "PRJNA1170571", "dataset_uri": "https://www.ncbi.nlm.nih.gov/bioproject/PRJNA1170571", "dataset_description": "Raw sequence reads", "dataset_file_name": null}]</t>
-  </si>
-  <si>
     <t>biogrid_6</t>
   </si>
   <si>
@@ -677,6 +668,42 @@
   </si>
   <si>
     <t>Genome-Scale CRISPRa Screen for Response to Cholera-Diphtheria Toxin</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Panea RI (2019) - 2-PMID31558468", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=2363", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Panea RI (2019) - 5-PMID31558468", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=2366", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Gilbert LA (2014) - 1-PMID25307932", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=1161", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Gilbert LA (2014) - 3-PMID25307932", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=6", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Panea RI (2019) - 6-PMID31558468", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=2367", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Gilbert LA (2014) - 2-PMID25307932", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=5", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Panea RI (2019) - 4-PMID31558468", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=2365", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "PRJNA1170571", "dataset_uri": "https://www.ncbi.nlm.nih.gov/bioproject/PRJNA1170571", "dataset_description": "Raw sequence reads", "dataset_file_name": null},{"dataset_accession": "Chen Z (2024) - 1-PMID39547224", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=2373", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Panea RI (2019) - 1-PMID31558468", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=2362", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Gilbert LA (2014) - 4-PMID25307932", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=1162", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>[{"dataset_accession": "Panea RI (2019) - 3-PMID31558468", "dataset_uri": "https://orcs.thebiogrid.org/Download?type=screen&amp;id=2364", "dataset_description": "Scores", "dataset_file_name": null}]</t>
+  </si>
+  <si>
+    <t>Jonathan S. Weissman</t>
   </si>
 </sst>
 </file>
@@ -1765,8 +1792,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A129C7D-22E4-1E47-A2F3-406D75945C4B}">
   <dimension ref="A1:CD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="BR12" sqref="BR12"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2104,22 +2132,22 @@
     </row>
     <row r="2" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
         <v>83</v>
       </c>
       <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" t="s">
         <v>128</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>129</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>130</v>
-      </c>
-      <c r="G2" t="s">
-        <v>131</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>86</v>
@@ -2135,49 +2163,49 @@
         <v>89</v>
       </c>
       <c r="M2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N2" t="s">
         <v>132</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>133</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>134</v>
-      </c>
-      <c r="P2" t="s">
-        <v>135</v>
       </c>
       <c r="Q2" t="s">
         <v>94</v>
       </c>
       <c r="S2" t="s">
+        <v>135</v>
+      </c>
+      <c r="U2" t="s">
         <v>136</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>137</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>138</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>139</v>
-      </c>
-      <c r="X2" t="s">
-        <v>140</v>
       </c>
       <c r="Y2">
         <v>2014</v>
       </c>
       <c r="Z2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AA2" t="s">
-        <v>153</v>
+        <v>227</v>
       </c>
       <c r="AB2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC2" t="s">
         <v>141</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>142</v>
       </c>
       <c r="AD2">
         <v>15319</v>
@@ -2192,22 +2220,22 @@
         <v>103</v>
       </c>
       <c r="AH2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>144</v>
       </c>
-      <c r="AI2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AL2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN2" t="s">
         <v>145</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AP2" t="s">
         <v>145</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>146</v>
       </c>
       <c r="AR2" t="s">
         <v>109</v>
@@ -2216,10 +2244,10 @@
         <v>109</v>
       </c>
       <c r="AV2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AW2" t="s">
         <v>147</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>148</v>
       </c>
       <c r="AX2" t="s">
         <v>112</v>
@@ -2228,10 +2256,10 @@
         <v>113</v>
       </c>
       <c r="BB2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BD2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BE2">
         <v>3</v>
@@ -2267,21 +2295,21 @@
         <v>122</v>
       </c>
       <c r="CD2" t="s">
-        <v>123</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="s">
         <v>128</v>
-      </c>
-      <c r="E3" t="s">
-        <v>129</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>86</v>
@@ -2297,49 +2325,49 @@
         <v>89</v>
       </c>
       <c r="M3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N3" t="s">
         <v>132</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>133</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>134</v>
-      </c>
-      <c r="P3" t="s">
-        <v>135</v>
       </c>
       <c r="Q3" t="s">
         <v>94</v>
       </c>
       <c r="S3" t="s">
+        <v>135</v>
+      </c>
+      <c r="U3" t="s">
         <v>136</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>137</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>138</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>139</v>
-      </c>
-      <c r="X3" t="s">
-        <v>140</v>
       </c>
       <c r="Y3">
         <v>2014</v>
       </c>
       <c r="Z3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AA3" t="s">
-        <v>153</v>
+        <v>227</v>
       </c>
       <c r="AB3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC3" t="s">
         <v>151</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>152</v>
       </c>
       <c r="AD3">
         <v>15350</v>
@@ -2354,22 +2382,22 @@
         <v>103</v>
       </c>
       <c r="AH3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AJ3" t="s">
         <v>144</v>
       </c>
-      <c r="AI3" t="s">
-        <v>143</v>
-      </c>
-      <c r="AJ3" t="s">
+      <c r="AL3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN3" t="s">
         <v>145</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AP3" t="s">
         <v>145</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>146</v>
       </c>
       <c r="AR3" t="s">
         <v>109</v>
@@ -2378,10 +2406,10 @@
         <v>109</v>
       </c>
       <c r="AV3" t="s">
+        <v>146</v>
+      </c>
+      <c r="AW3" t="s">
         <v>147</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>148</v>
       </c>
       <c r="AX3" t="s">
         <v>112</v>
@@ -2390,10 +2418,10 @@
         <v>113</v>
       </c>
       <c r="BB3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BD3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BE3">
         <v>3</v>
@@ -2429,12 +2457,12 @@
         <v>122</v>
       </c>
       <c r="CD3" t="s">
-        <v>123</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
         <v>83</v>
@@ -2465,10 +2493,10 @@
         <v>91</v>
       </c>
       <c r="O4" t="s">
+        <v>124</v>
+      </c>
+      <c r="P4" t="s">
         <v>125</v>
-      </c>
-      <c r="P4" t="s">
-        <v>126</v>
       </c>
       <c r="Q4" t="s">
         <v>94</v>
@@ -2498,7 +2526,7 @@
         <v>101</v>
       </c>
       <c r="AB4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AC4" t="s">
         <v>102</v>
@@ -2591,7 +2619,7 @@
         <v>122</v>
       </c>
       <c r="CD4" t="s">
-        <v>123</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:82" x14ac:dyDescent="0.2">
@@ -2660,10 +2688,10 @@
         <v>101</v>
       </c>
       <c r="AB5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AC5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AD5">
         <v>2777</v>
@@ -2753,12 +2781,12 @@
         <v>122</v>
       </c>
       <c r="CD5" t="s">
-        <v>123</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
@@ -2789,13 +2817,13 @@
         <v>91</v>
       </c>
       <c r="O6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="P6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="S6" t="s">
         <v>95</v>
@@ -2822,10 +2850,10 @@
         <v>101</v>
       </c>
       <c r="AB6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AC6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AD6">
         <v>2777</v>
@@ -2915,12 +2943,12 @@
         <v>122</v>
       </c>
       <c r="CD6" t="s">
-        <v>123</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s">
         <v>83</v>
@@ -2951,19 +2979,19 @@
         <v>91</v>
       </c>
       <c r="O7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="S7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="V7" t="s">
         <v>97</v>
@@ -2984,10 +3012,10 @@
         <v>101</v>
       </c>
       <c r="AB7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AC7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AD7">
         <v>2777</v>
@@ -3077,12 +3105,12 @@
         <v>122</v>
       </c>
       <c r="CD7" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>83</v>
@@ -3113,19 +3141,19 @@
         <v>91</v>
       </c>
       <c r="O8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="P8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="S8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="V8" t="s">
         <v>97</v>
@@ -3146,10 +3174,10 @@
         <v>101</v>
       </c>
       <c r="AB8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC8" t="s">
         <v>171</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>173</v>
       </c>
       <c r="AD8">
         <v>2777</v>
@@ -3239,12 +3267,12 @@
         <v>122</v>
       </c>
       <c r="CD8" t="s">
-        <v>123</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B9" t="s">
         <v>83</v>
@@ -3275,19 +3303,19 @@
         <v>91</v>
       </c>
       <c r="O9" t="s">
+        <v>174</v>
+      </c>
+      <c r="P9" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>157</v>
+      </c>
+      <c r="S9" t="s">
         <v>176</v>
       </c>
-      <c r="P9" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>159</v>
-      </c>
-      <c r="S9" t="s">
-        <v>178</v>
-      </c>
       <c r="U9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="V9" t="s">
         <v>97</v>
@@ -3308,10 +3336,10 @@
         <v>101</v>
       </c>
       <c r="AB9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AC9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AD9">
         <v>2777</v>
@@ -3401,12 +3429,12 @@
         <v>122</v>
       </c>
       <c r="CD9" t="s">
-        <v>123</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
@@ -3415,13 +3443,13 @@
         <v>84</v>
       </c>
       <c r="E10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G10" t="s">
         <v>182</v>
-      </c>
-      <c r="F10" t="s">
-        <v>183</v>
-      </c>
-      <c r="G10" t="s">
-        <v>184</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>86</v>
@@ -3431,22 +3459,22 @@
         <v>87</v>
       </c>
       <c r="K10" t="s">
+        <v>183</v>
+      </c>
+      <c r="L10" t="s">
+        <v>184</v>
+      </c>
+      <c r="M10" t="s">
         <v>185</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>186</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>187</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>188</v>
-      </c>
-      <c r="O10" t="s">
-        <v>189</v>
-      </c>
-      <c r="P10" t="s">
-        <v>190</v>
       </c>
       <c r="Q10" t="s">
         <v>94</v>
@@ -3455,31 +3483,31 @@
         <v>95</v>
       </c>
       <c r="U10" t="s">
+        <v>189</v>
+      </c>
+      <c r="V10" t="s">
+        <v>190</v>
+      </c>
+      <c r="W10" t="s">
+        <v>192</v>
+      </c>
+      <c r="X10" t="s">
         <v>191</v>
       </c>
-      <c r="V10" t="s">
-        <v>192</v>
-      </c>
-      <c r="W10" t="s">
+      <c r="Y10">
+        <v>2024</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>193</v>
+      </c>
+      <c r="AA10" t="s">
         <v>194</v>
       </c>
-      <c r="X10" t="s">
-        <v>193</v>
-      </c>
-      <c r="Y10">
-        <v>20224</v>
-      </c>
-      <c r="Z10" t="s">
+      <c r="AB10" t="s">
         <v>195</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AC10" t="s">
         <v>196</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>197</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>198</v>
       </c>
       <c r="AD10">
         <v>18053</v>
@@ -3488,7 +3516,7 @@
         <v>38000000</v>
       </c>
       <c r="AF10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AG10" s="2" t="s">
         <v>105</v>
@@ -3500,16 +3528,16 @@
         <v>105</v>
       </c>
       <c r="AJ10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN10" t="s">
         <v>145</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AP10" t="s">
         <v>145</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>146</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>146</v>
       </c>
       <c r="AR10" t="s">
         <v>109</v>
@@ -3518,10 +3546,10 @@
         <v>109</v>
       </c>
       <c r="AV10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="AW10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AX10" t="s">
         <v>112</v>
@@ -3533,7 +3561,7 @@
         <v>114</v>
       </c>
       <c r="BD10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="BE10">
         <v>3</v>
@@ -3557,33 +3585,33 @@
         <v>119</v>
       </c>
       <c r="BT10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="BV10" t="s">
         <v>121</v>
       </c>
       <c r="BX10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="BZ10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="CD10" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
         <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>86</v>
@@ -3599,49 +3627,49 @@
         <v>89</v>
       </c>
       <c r="M11" t="s">
+        <v>131</v>
+      </c>
+      <c r="N11" t="s">
         <v>132</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>133</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>134</v>
-      </c>
-      <c r="P11" t="s">
-        <v>135</v>
       </c>
       <c r="Q11" t="s">
         <v>94</v>
       </c>
       <c r="S11" t="s">
+        <v>135</v>
+      </c>
+      <c r="U11" t="s">
         <v>136</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>137</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>138</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>139</v>
-      </c>
-      <c r="X11" t="s">
-        <v>140</v>
       </c>
       <c r="Y11">
         <v>2014</v>
       </c>
       <c r="Z11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AA11" t="s">
-        <v>153</v>
+        <v>227</v>
       </c>
       <c r="AB11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AC11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AD11">
         <v>15977</v>
@@ -3656,22 +3684,22 @@
         <v>103</v>
       </c>
       <c r="AH11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AI11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AJ11" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN11" t="s">
         <v>145</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AP11" t="s">
         <v>145</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>146</v>
-      </c>
-      <c r="AP11" t="s">
-        <v>146</v>
       </c>
       <c r="AR11" t="s">
         <v>109</v>
@@ -3680,10 +3708,10 @@
         <v>109</v>
       </c>
       <c r="AV11" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AW11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AX11" t="s">
         <v>112</v>
@@ -3692,10 +3720,10 @@
         <v>113</v>
       </c>
       <c r="BB11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="BD11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BE11">
         <v>3</v>
@@ -3731,27 +3759,27 @@
         <v>122</v>
       </c>
       <c r="CD11" t="s">
-        <v>123</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B12" t="s">
         <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>86</v>
@@ -3767,49 +3795,49 @@
         <v>89</v>
       </c>
       <c r="M12" t="s">
+        <v>131</v>
+      </c>
+      <c r="N12" t="s">
         <v>132</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>133</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>134</v>
-      </c>
-      <c r="P12" t="s">
-        <v>135</v>
       </c>
       <c r="Q12" t="s">
         <v>94</v>
       </c>
       <c r="S12" t="s">
+        <v>135</v>
+      </c>
+      <c r="U12" t="s">
         <v>136</v>
       </c>
-      <c r="U12" t="s">
+      <c r="V12" t="s">
         <v>137</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>138</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>139</v>
-      </c>
-      <c r="X12" t="s">
-        <v>140</v>
       </c>
       <c r="Y12">
         <v>2014</v>
       </c>
       <c r="Z12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AA12" t="s">
-        <v>153</v>
+        <v>227</v>
       </c>
       <c r="AB12" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="AC12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="AD12">
         <v>15977</v>
@@ -3824,22 +3852,22 @@
         <v>103</v>
       </c>
       <c r="AH12" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AI12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AJ12" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN12" t="s">
         <v>145</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="AP12" t="s">
         <v>145</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>146</v>
-      </c>
-      <c r="AP12" t="s">
-        <v>146</v>
       </c>
       <c r="AR12" t="s">
         <v>109</v>
@@ -3848,10 +3876,10 @@
         <v>109</v>
       </c>
       <c r="AV12" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AW12" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AX12" t="s">
         <v>112</v>
@@ -3860,10 +3888,10 @@
         <v>113</v>
       </c>
       <c r="BB12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="BD12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BE12">
         <v>3</v>
@@ -3899,7 +3927,7 @@
         <v>122</v>
       </c>
       <c r="CD12" t="s">
-        <v>123</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added MIT license for biogrid studies
</commit_message>
<xml_diff>
--- a/data_exploration/CRISPR/crispr_studies.xlsx
+++ b/data_exploration/CRISPR/crispr_studies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zakirov/Documents/GitHub/PerturbationCatalogue/data_exploration/CRISPR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23162C9-4BC0-764D-A702-C70E7795C2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EA277E-29CE-094F-9752-C13F99073E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="2440" windowWidth="28040" windowHeight="17440" xr2:uid="{65AE61D5-2EF1-1F4C-8D97-BC1AA3C27BF4}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="232">
   <si>
     <t>dataset_id</t>
   </si>
@@ -704,13 +704,25 @@
   </si>
   <si>
     <t>Jonathan S. Weissman</t>
+  </si>
+  <si>
+    <t>license_label</t>
+  </si>
+  <si>
+    <t>license_id</t>
+  </si>
+  <si>
+    <t>MIT License</t>
+  </si>
+  <si>
+    <t>SWO:9000074</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -841,6 +853,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1380,12 +1398,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{39B4455B-CE12-364D-83A3-3F367B4C8ED5}" name="Table1" displayName="Table1" ref="A1:CD11" totalsRowShown="0">
-  <autoFilter ref="A1:CD11" xr:uid="{39B4455B-CE12-364D-83A3-3F367B4C8ED5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{39B4455B-CE12-364D-83A3-3F367B4C8ED5}" name="Table1" displayName="Table1" ref="A1:CF11" totalsRowShown="0">
+  <autoFilter ref="A1:CF11" xr:uid="{39B4455B-CE12-364D-83A3-3F367B4C8ED5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CD9">
     <sortCondition ref="X1:X9"/>
   </sortState>
-  <tableColumns count="82">
+  <tableColumns count="84">
     <tableColumn id="1" xr3:uid="{FE579D00-969B-2F4B-9AF9-9C98E176F2C3}" name="dataset_id"/>
     <tableColumn id="2" xr3:uid="{ADBB44E8-65BD-8C44-B6DF-3827A4FD1885}" name="data_modality"/>
     <tableColumn id="3" xr3:uid="{F82B393E-7236-E048-9087-9A9C0210C295}" name="perturbation_type_label"/>
@@ -1468,6 +1486,8 @@
     <tableColumn id="81" xr3:uid="{C8B46FD7-001F-5A43-B74E-F232DD60157A}" name="reference_genome_label"/>
     <tableColumn id="80" xr3:uid="{7EAEE04A-29ED-B046-8BF6-F8D7C25A3E9E}" name="reference_genome_id"/>
     <tableColumn id="82" xr3:uid="{F86B596B-DED8-9948-A57E-CC5455907A73}" name="associated_datasets"/>
+    <tableColumn id="83" xr3:uid="{0732A113-4B93-5243-8025-45BB948323BA}" name="license_label"/>
+    <tableColumn id="84" xr3:uid="{85C63EFC-3D94-814E-90D0-282BD4120197}" name="license_id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1790,11 +1810,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A129C7D-22E4-1E47-A2F3-406D75945C4B}">
-  <dimension ref="A1:CD12"/>
+  <dimension ref="A1:CF12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA5" sqref="AA5"/>
+      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CD10" sqref="CD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1879,10 +1899,12 @@
     <col min="79" max="79" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="85" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2129,8 +2151,14 @@
       <c r="CD1" t="s">
         <v>81</v>
       </c>
+      <c r="CE1" t="s">
+        <v>228</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -2297,8 +2325,14 @@
       <c r="CD2" t="s">
         <v>218</v>
       </c>
+      <c r="CE2" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -2459,8 +2493,14 @@
       <c r="CD3" t="s">
         <v>221</v>
       </c>
+      <c r="CE3" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -2621,8 +2661,14 @@
       <c r="CD4" t="s">
         <v>224</v>
       </c>
+      <c r="CE4" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF4" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="5" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -2783,8 +2829,14 @@
       <c r="CD5" t="s">
         <v>216</v>
       </c>
+      <c r="CE5" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF5" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -2945,8 +2997,14 @@
       <c r="CD6" t="s">
         <v>226</v>
       </c>
+      <c r="CE6" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF6" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -3107,8 +3165,14 @@
       <c r="CD7" t="s">
         <v>222</v>
       </c>
+      <c r="CE7" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF7" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -3269,8 +3333,14 @@
       <c r="CD8" t="s">
         <v>217</v>
       </c>
+      <c r="CE8" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF8" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>173</v>
       </c>
@@ -3431,8 +3501,14 @@
       <c r="CD9" t="s">
         <v>220</v>
       </c>
+      <c r="CE9" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF9" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>179</v>
       </c>
@@ -3599,8 +3675,14 @@
       <c r="CD10" t="s">
         <v>223</v>
       </c>
+      <c r="CE10" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF10" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>204</v>
       </c>
@@ -3761,8 +3843,14 @@
       <c r="CD11" t="s">
         <v>219</v>
       </c>
+      <c r="CE11" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF11" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -3931,6 +4019,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">

</xml_diff>